<commit_message>
Curso 02 | Desafio 04 | Feito
</commit_message>
<xml_diff>
--- a/Formacao-VBA-Curso-02/Projects/Modulo-04/planilha-visualizacao-contas-recentes.xlsx
+++ b/Formacao-VBA-Curso-02/Projects/Modulo-04/planilha-visualizacao-contas-recentes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\Work_Space\ALURA\Excel\excel-funcoes-material-inicial\Projects\Modulo-01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\Work_Space\ALURA\Excel\Formacao-VBA-Curso-02\Projects\Modulo-04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E9D75D-FC9A-42AA-A51F-77C08C83DAF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449FB965-E1D6-4F60-80E7-15394DC63DCD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -216,9 +216,6 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -246,6 +243,9 @@
     <xf numFmtId="44" fontId="0" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -530,171 +530,171 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>44177</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="12">
+      <c r="B3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="11">
         <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>44147</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="13">
+      <c r="B4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="12">
         <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>44116</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="13">
+      <c r="B5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12">
         <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>44086</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="13">
+      <c r="B6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="12">
         <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>44055</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="13">
+      <c r="B7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="12">
         <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>44024</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="13">
+      <c r="B8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="12">
         <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>43994</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="13">
+      <c r="B9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="12">
         <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>43963</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="13">
+      <c r="B10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="12">
         <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>43933</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="13">
+      <c r="B11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="12">
         <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>43902</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="13">
+      <c r="B12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="12">
         <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>43873</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="13">
+      <c r="B13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="12">
         <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
+      <c r="A14" s="6">
         <v>43842</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="14">
+      <c r="B14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="13">
         <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="14"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C14">
@@ -704,6 +704,12 @@
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="textLength" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Atenção" error="Tente digitar um nome de conta com no máximo 20 letras." promptTitle="Atenção" prompt="Tente digitar um nome de conta com no máximo 20 letras." sqref="B2:B14" xr:uid="{6E4BDD5D-3FA1-4ED7-8B3A-AAB06226B822}">
+      <formula1>0</formula1>
+      <formula2>20</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>